<commit_message>
Actualización de Diagrama, Esquematico y Listado de materiales.
</commit_message>
<xml_diff>
--- a/Listado de Materiales.xlsx
+++ b/Listado de Materiales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Estudio\UdeA\2024-2\Informatica II\Laboratorios\Desafio 1 2024-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82067C6-0EDB-46F5-B27B-B03791E3D4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F796EC8-E267-48CD-89B0-D567ACA1B813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0FE3618A-84EF-4AF0-9493-2F9F7AB07500}"/>
+    <workbookView xWindow="-24120" yWindow="-990" windowWidth="24240" windowHeight="13140" xr2:uid="{0FE3618A-84EF-4AF0-9493-2F9F7AB07500}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Materiales" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -40,18 +40,12 @@
     <t>FUNC1</t>
   </si>
   <si>
-    <t>2 Hz, 1 V, 0 V, Seno Generador de función</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
     <t xml:space="preserve"> LCD 16 x 2</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Pulsador</t>
   </si>
   <si>
@@ -71,13 +65,25 @@
   </si>
   <si>
     <t>10 kΩ Resistencia</t>
+  </si>
+  <si>
+    <t>1 Hz, 2 V, 0 V, Seno Generador de función</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>S inicio</t>
+  </si>
+  <si>
+    <t>S captura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,13 +226,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -409,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -534,6 +533,32 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -584,12 +609,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -967,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA4B70A-CBFC-4F6E-9B8B-DA3C35BD0087}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,84 +1031,104 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="C10" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>